<commit_message>
Added functions to sunai_challenge and passed tests
</commit_message>
<xml_diff>
--- a/test/cases/subfolder/dummy.xlsx
+++ b/test/cases/subfolder/dummy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">id_i</t>
   </si>
@@ -28,10 +28,85 @@
     <t xml:space="preserve">fecha_im</t>
   </si>
   <si>
+    <t xml:space="preserve">id_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apparent_power_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_current_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_voltage_phase1_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_voltage_phase2_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_voltage_phase3_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc_current_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc_power_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc_voltage_im</t>
+  </si>
+  <si>
     <t xml:space="preserve">active_energy_im</t>
   </si>
   <si>
     <t xml:space="preserve">active_power_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reactive_power_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frequency_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature_internal_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature_external_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature_heatsink_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isolation_resistance_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power_factor_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imputed_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_current_phase1_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_current_phase2_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac_current_phase3_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cos_phi_im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod_alerta_inversor_medicion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha_recepcion_inversor_medicion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha_act_inversor_medicion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imputado_inversor_medicion</t>
   </si>
 </sst>
 </file>
@@ -107,16 +182,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -137,15 +208,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -161,18 +233,96 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>44882</v>
+      <c r="B2" s="1" t="n">
+        <v>44883</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>321</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>123456789</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>987654321</v>
       </c>
     </row>

</xml_diff>